<commit_message>
add: report about confidence intervals in statistic
</commit_message>
<xml_diff>
--- a/lab1/parProg_lab1/parProg_lab1/statistic_lab2.xlsx
+++ b/lab1/parProg_lab1/parProg_lab1/statistic_lab2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3_year\labs\paralProgramming\lab1\parProg_lab1\parProg_lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3640579-2E09-4C39-9A81-32021FE1217E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDC222C-3D55-4030-B229-ED0B41AE861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,10 +83,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1225,8 +1225,8 @@
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1242,7 +1242,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3093720"/>
-          <a:ext cx="4213860" cy="1424940"/>
+          <a:ext cx="4213860" cy="1714500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1278,7 +1278,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="ru-RU" sz="1100"/>
-            <a:t>вывод: были перемножены матрицы разных размеров (200х200, 400х400, 800х800), измерено время за которое происходит умножнние, в зависимости от количества выделенных потоков(1,2,4,8,16). Видно что при выделении 16 потоков время сократилось по сравнению с 1 потоком примерно в 5-6 раз для матрицы 800х800, для матрицы 400х400 примерно в 6-7 раз, дальнейшее увеличение потоков ускоряет работу лишь немного</a:t>
+            <a:t>вывод: были перемножены матрицы разных размеров (200х200, 400х400, 800х800), измерено время за которое происходит умножнние, в зависимости от количества выделенных потоков(1,2,4,8,16). Видно что при выделении 16 потоков время сократилось по сравнению с 1 потоком примерно в 5-6 раз для матрицы 800х800, для матрицы 400х400 примерно в 6-7 раз, дальнейшее увеличение потоков ускоряет работу лишь немного.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>доверительные интервалы +- 10% от указанного времени выполнения</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1568,15 +1574,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1755,49 +1761,49 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>